<commit_message>
Added toe output to single file
</commit_message>
<xml_diff>
--- a/Notebooks/Constanta Phase III/Input data/first_test_data_phase_III.xlsx
+++ b/Notebooks/Constanta Phase III/Input data/first_test_data_phase_III.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JY6\github\breakwater\Notebooks\Constanta Phase III\Input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32C80FD0-2561-4A4C-89C3-C7F1C47B15F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{05D0C7BF-DF22-4B80-94B7-C721BF9AD75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{06ED436A-2CC0-4489-A506-29F94518B839}"/>
   </bookViews>
@@ -26,9 +26,9 @@
     <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
-    <definedName name="Lt">'[1]Input_Project specific'!$E$20</definedName>
-    <definedName name="rho_r">'[1]Input_Project specific'!$E$3</definedName>
-    <definedName name="weight_check">'[1]Input_Project specific'!$E$19</definedName>
+    <definedName name="Lt">'Input_Project specific'!$E$20</definedName>
+    <definedName name="rho_r">'Input_Project specific'!$E$3</definedName>
+    <definedName name="weight_check">'Input_Project specific'!$E$19</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -2269,11 +2269,6 @@
             <v>Minimal</v>
           </cell>
         </row>
-        <row r="20">
-          <cell r="E20">
-            <v>1.82</v>
-          </cell>
-        </row>
       </sheetData>
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
@@ -4240,7 +4235,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31169,12 +31164,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -31407,15 +31399,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A37F9B0-FB51-4EBC-8606-1AACB4773553}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A202D3EF-E74A-4B50-BD9D-588EBDA690CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="13eb6276-85db-4ef3-a671-167ab07ac255"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="fc9abb88-5dc8-4425-a823-e2986ac3f199"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -31440,18 +31444,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A202D3EF-E74A-4B50-BD9D-588EBDA690CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A37F9B0-FB51-4EBC-8606-1AACB4773553}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="13eb6276-85db-4ef3-a671-167ab07ac255"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="fc9abb88-5dc8-4425-a823-e2986ac3f199"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>